<commit_message>
Actualización automática 2025-05-27 16:15:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>-199.99</v>
+        <v>966.41</v>
       </c>
     </row>
     <row r="9">
@@ -1901,7 +1901,7 @@
         <v>4071.09</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>2239.85</v>
       </c>
     </row>
     <row r="14">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>19412.65</v>
+        <v>22818.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-27 16:20:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1901,7 +1901,7 @@
         <v>4071.09</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>2239.85</v>
+        <v>6262.37</v>
       </c>
     </row>
     <row r="14">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>22818.9</v>
+        <v>26841.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-27 16:25:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1901,7 +1901,7 @@
         <v>4071.09</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>6262.37</v>
+        <v>9034.549999999999</v>
       </c>
     </row>
     <row r="14">
@@ -2093,7 +2093,7 @@
         <v>4830.33</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>3379.94</v>
+        <v>5131.72</v>
       </c>
     </row>
     <row r="22">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>26841.42</v>
+        <v>31365.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-28 13:40:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1829,7 +1829,7 @@
         <v>2112.18</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>9479.01</v>
+        <v>9416.799999999999</v>
       </c>
     </row>
     <row r="11">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>31365.38</v>
+        <v>31303.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-29 10:40:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1581,7 +1581,7 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1733,7 +1733,7 @@
         <v>8024.83</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>2935.25</v>
+        <v>6839.4</v>
       </c>
     </row>
     <row r="7">
@@ -2093,7 +2093,7 @@
         <v>4830.33</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>5131.72</v>
+        <v>15564.83</v>
       </c>
     </row>
     <row r="22">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>31303.17</v>
+        <v>45640.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-30 11:55:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1781,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>966.41</v>
+        <v>7010.57</v>
       </c>
     </row>
     <row r="9">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>45640.43</v>
+        <v>51684.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-05-30 17:40:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -961,10 +961,10 @@
         <v>9002.940000000001</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>124.22</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>2189.72</v>
+        <v>2438.55</v>
       </c>
     </row>
     <row r="11">
@@ -1548,7 +1548,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>1 de 20</t>
+          <t>2 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -1829,7 +1829,7 @@
         <v>2112.18</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>11192.66</v>
+        <v>11565.71</v>
       </c>
     </row>
     <row r="11">
@@ -2107,7 +2107,7 @@
         <v>25096.15</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>54296.05</v>
+        <v>54669.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-09 09:45:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -2205,9 +2205,9 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2617,13 +2617,13 @@
         <v>342</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>-124.22</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>342</v>
+        <v>466.22</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>0</v>
+        <v>-0.3632163742690058</v>
       </c>
     </row>
     <row r="18">
@@ -2641,13 +2641,13 @@
         <v>2800</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0</v>
+        <v>-248.83</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>2800</v>
+        <v>3048.83</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>0</v>
+        <v>-0.08886785714285715</v>
       </c>
     </row>
     <row r="19">
@@ -2660,13 +2660,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>-373.05</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50387.19762291768</v>
+        <v>50760.24762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0</v>
+        <v>-0.007403666359693026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-09 14:35:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>43.54</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="F22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="G22" s="4" t="inlineStr">
@@ -1863,7 +1863,7 @@
         <v>11565.71</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-373.05</v>
+        <v>-329.51</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>7000</v>
@@ -2177,7 +2177,7 @@
         <v>54669.1</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>-373.05</v>
+        <v>-329.51</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>
@@ -2206,7 +2206,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2353,13 +2353,13 @@
         <v>106.82</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>43.54</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>106.82</v>
+        <v>63.27999999999999</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>0.4076015727391875</v>
       </c>
     </row>
     <row r="7">
@@ -2660,13 +2660,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>-373.05</v>
+        <v>-329.51</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50760.24762291768</v>
+        <v>50716.70762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>-0.007403666359693026</v>
+        <v>-0.006539557973951076</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-16 17:20:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1718,7 +1718,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0</v>
+        <v>274.75</v>
       </c>
       <c r="E21" s="2" t="n">
         <v>0</v>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="E22" s="4" t="inlineStr">
@@ -2444,7 +2444,7 @@
         <v>15564.83</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>274.75</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>4000</v>
@@ -2461,7 +2461,7 @@
         <v>54669.1</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>-329.51</v>
+        <v>-54.75999999999999</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>
@@ -2565,13 +2565,13 @@
         <v>4168.07156573679</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0</v>
+        <v>274.75</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4168.07156573679</v>
+        <v>3893.32156573679</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0</v>
+        <v>0.0659177741233031</v>
       </c>
     </row>
     <row r="4">
@@ -2944,13 +2944,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>-329.51</v>
+        <v>-54.75999999999999</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50716.70762291769</v>
+        <v>50441.95762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>-0.006539557973951076</v>
+        <v>-0.001086783996399383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-18 11:45:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0</v>
+        <v>45.91</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>45.91</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>6500</v>
@@ -2461,7 +2461,7 @@
         <v>54669.1</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>-54.75999999999999</v>
+        <v>-8.849999999999994</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>
@@ -2877,13 +2877,13 @@
         <v>29532.44</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0</v>
+        <v>45.91</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>29532.44</v>
+        <v>29486.53</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0</v>
+        <v>0.001554561695545644</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>-54.75999999999999</v>
+        <v>-8.849999999999966</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50441.95762291769</v>
+        <v>50396.04762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>-0.001086783996399383</v>
+        <v>-0.0001756398533260502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-21 14:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0</v>
+        <v>3228.67</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>2 de 20</t>
+          <t>3 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2201,7 +2201,7 @@
         <v>1565.15</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0</v>
+        <v>3228.67</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>6000</v>
@@ -2461,7 +2461,7 @@
         <v>54669.1</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>168.56</v>
+        <v>3397.23</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>
@@ -2877,13 +2877,13 @@
         <v>29532.44</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>223.32</v>
+        <v>3451.99</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>29309.12</v>
+        <v>26080.45</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.007561854015448774</v>
+        <v>0.1168880729123635</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>168.56</v>
+        <v>3397.23</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50218.63762291768</v>
+        <v>46989.96762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.003345294200750184</v>
+        <v>0.0674224834932045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-23 16:10:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1397,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="2" t="n">
-        <v>0</v>
+        <v>431.64</v>
       </c>
       <c r="R15" s="2" t="n">
         <v>0</v>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="Q22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="R22" s="4" t="inlineStr">
@@ -2282,7 +2282,7 @@
         <v>288.17</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>0</v>
+        <v>431.64</v>
       </c>
       <c r="G15" s="2" t="n">
         <v>400</v>
@@ -2461,7 +2461,7 @@
         <v>54669.1</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>3409.33</v>
+        <v>3840.97</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>
@@ -2829,13 +2829,13 @@
         <v>483</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>431.64</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>483</v>
+        <v>51.36000000000001</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0</v>
+        <v>0.8936645962732919</v>
       </c>
     </row>
     <row r="15">
@@ -2944,13 +2944,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3409.33</v>
+        <v>3840.970000000001</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46977.86762291769</v>
+        <v>46546.22762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.06766262385763899</v>
+        <v>0.07622908558528381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-06-25 08:30:10
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1070,10 +1070,10 @@
         <v>43.54</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0</v>
+        <v>3756.6</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>0</v>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0</v>
+        <v>1128.6</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0</v>
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>0</v>
+        <v>2215.7</v>
       </c>
       <c r="R18" s="2" t="n">
         <v>0</v>
@@ -1791,52 +1791,52 @@
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
+          <t>2 de 20</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>1 de 20</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
+        <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="I22" s="4" t="inlineStr">
+      <c r="K22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="J22" s="4" t="inlineStr">
+      <c r="L22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="K22" s="4" t="inlineStr">
+      <c r="M22" s="4" t="inlineStr">
+        <is>
+          <t>4 de 20</t>
+        </is>
+      </c>
+      <c r="N22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="L22" s="4" t="inlineStr">
+      <c r="O22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="M22" s="4" t="inlineStr">
-        <is>
-          <t>4 de 20</t>
-        </is>
-      </c>
-      <c r="N22" s="4" t="inlineStr">
+      <c r="P22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="O22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="P22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
       <c r="Q22" s="4" t="inlineStr">
         <is>
-          <t>1 de 20</t>
+          <t>2 de 20</t>
         </is>
       </c>
       <c r="R22" s="4" t="inlineStr">
@@ -2147,7 +2147,7 @@
         <v>11565.71</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>-329.51</v>
+        <v>4687.09</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>7000</v>
@@ -2201,7 +2201,7 @@
         <v>1565.15</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>3228.67</v>
+        <v>4357.27</v>
       </c>
       <c r="G12" s="2" t="n">
         <v>6000</v>
@@ -2363,7 +2363,7 @@
         <v>290.56</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>2215.7</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>4000</v>
@@ -2461,7 +2461,7 @@
         <v>54669.1</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>3840.97</v>
+        <v>12201.87</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>
@@ -2661,13 +2661,13 @@
         <v>1800</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>4885.2</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1800</v>
+        <v>-3085.2</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>2.714</v>
       </c>
     </row>
     <row r="8">
@@ -2685,13 +2685,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>625</v>
+        <v>-635</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>2.016</v>
       </c>
     </row>
     <row r="9">
@@ -2829,13 +2829,13 @@
         <v>483</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>431.64</v>
+        <v>2647.34</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>51.36000000000001</v>
+        <v>-2164.34</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.8936645962732919</v>
+        <v>5.481035196687371</v>
       </c>
     </row>
     <row r="15">
@@ -2944,13 +2944,13 @@
         <v>50387.19762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3840.970000000001</v>
+        <v>12201.87</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46546.22762291769</v>
+        <v>38185.32762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.07622908558528381</v>
+        <v>0.2421621081472927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-02 17:15:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -977,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>0</v>
+        <v>625.86</v>
       </c>
       <c r="R8" s="2" t="n">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0</v>
+        <v>6678.14</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -1816,27 +1816,27 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
+          <t>2 de 20</t>
+        </is>
+      </c>
+      <c r="N22" s="4" t="inlineStr">
+        <is>
+          <t>0 de 20</t>
+        </is>
+      </c>
+      <c r="O22" s="4" t="inlineStr">
+        <is>
           <t>1 de 20</t>
         </is>
       </c>
-      <c r="N22" s="4" t="inlineStr">
+      <c r="P22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="O22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
-      <c r="P22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
       <c r="Q22" s="4" t="inlineStr">
         <is>
-          <t>1 de 20</t>
+          <t>2 de 20</t>
         </is>
       </c>
       <c r="R22" s="4" t="inlineStr">
@@ -2093,7 +2093,7 @@
         <v>211.12</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>625.86</v>
       </c>
       <c r="G8" s="2" t="n">
         <v>6000</v>
@@ -2309,7 +2309,7 @@
         <v>45.91</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>6678.14</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>6500</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>2941.14</v>
+        <v>10245.14</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>50400</v>

</xml_diff>

<commit_message>
Actualización automática 2025-07-04 17:10:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>3233.78</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>2 de 20</t>
+          <t>3 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2147,7 +2147,7 @@
         <v>4711.21</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>3233.78</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>6000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>10261.6</v>
+        <v>13495.38</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2489,7 +2489,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>7307.46</v>
+        <v>10541.24</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>36958.78</v>
+        <v>33725</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1650797537807593</v>
+        <v>0.23813271694185</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>10261.6</v>
+        <v>13495.38</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>55116.39762291768</v>
+        <v>51882.61762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1569580038101823</v>
+        <v>0.2064208218464818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-04 17:15:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="2" t="n">
-        <v>0</v>
+        <v>1368.58</v>
       </c>
       <c r="N18" s="2" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>3 de 20</t>
+          <t>4 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2363,7 +2363,7 @@
         <v>1935.16</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v>1368.58</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>4500</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>13495.38</v>
+        <v>14863.96</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>10541.24</v>
+        <v>11909.82</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>33725</v>
+        <v>32356.42</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.23813271694185</v>
+        <v>0.2690497318046439</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>13495.38</v>
+        <v>14863.96</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51882.61762291769</v>
+        <v>50514.03762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2064208218464818</v>
+        <v>0.2273541640986198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-04 17:20:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0</v>
+        <v>401.81</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0</v>
+        <v>3969.29</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
@@ -1776,47 +1776,47 @@
       </c>
       <c r="E22" s="4" t="inlineStr">
         <is>
+          <t>1 de 20</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="inlineStr">
+        <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="F22" s="4" t="inlineStr">
+      <c r="G22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>1 de 20</t>
+        </is>
+      </c>
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>1 de 20</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="H22" s="4" t="inlineStr">
+      <c r="K22" s="4" t="inlineStr">
+        <is>
+          <t>0 de 20</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
         <is>
           <t>1 de 20</t>
         </is>
       </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>4 de 20</t>
+          <t>5 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2012,7 +2012,7 @@
         <v>12.1</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0</v>
+        <v>4371.1</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>4000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>14863.96</v>
+        <v>19235.06</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2589,13 +2589,13 @@
         <v>513.831046659336</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>401.81</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>513.831046659336</v>
+        <v>112.021046659336</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0</v>
+        <v>0.7819885594931661</v>
       </c>
     </row>
     <row r="5">
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>11909.82</v>
+        <v>15879.11</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>32356.42</v>
+        <v>28387.13</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2690497318046439</v>
+        <v>0.3587182918630542</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>14863.96</v>
+        <v>19235.06</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>50514.03762291768</v>
+        <v>46142.93762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2273541640986198</v>
+        <v>0.2942130487223322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-08 17:00:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -905,7 +905,7 @@
         <v>86.56999999999999</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>629.3200000000001</v>
+        <v>697.36</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>0</v>
@@ -2066,7 +2066,7 @@
         <v>177.41</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>2228.69</v>
+        <v>2296.73</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1500</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>19235.06</v>
+        <v>19303.1</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>15879.11</v>
+        <v>15947.15</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>28387.13</v>
+        <v>28319.09</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.3587182918630542</v>
+        <v>0.3602553548708903</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>19235.06</v>
+        <v>19303.1</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46142.93762291769</v>
+        <v>46074.89762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2942130487223322</v>
+        <v>0.2952537658209566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 12:25:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>2472.77</v>
       </c>
       <c r="E6" s="2" t="n">
         <v>0</v>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>1451.52</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1771,52 +1771,52 @@
       </c>
       <c r="D22" s="4" t="inlineStr">
         <is>
+          <t>2 de 20</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
           <t>1 de 20</t>
         </is>
       </c>
-      <c r="E22" s="4" t="inlineStr">
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>0 de 20</t>
+        </is>
+      </c>
+      <c r="G22" s="4" t="inlineStr">
+        <is>
+          <t>0 de 20</t>
+        </is>
+      </c>
+      <c r="H22" s="4" t="inlineStr">
         <is>
           <t>1 de 20</t>
         </is>
       </c>
-      <c r="F22" s="4" t="inlineStr">
+      <c r="I22" s="4" t="inlineStr">
+        <is>
+          <t>1 de 20</t>
+        </is>
+      </c>
+      <c r="J22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr">
+      <c r="K22" s="4" t="inlineStr">
         <is>
           <t>0 de 20</t>
         </is>
       </c>
-      <c r="H22" s="4" t="inlineStr">
+      <c r="L22" s="4" t="inlineStr">
         <is>
           <t>1 de 20</t>
         </is>
       </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>5 de 20</t>
+          <t>6 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2039,7 +2039,7 @@
         <v>111.02</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>2472.77</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>4000</v>
@@ -2228,7 +2228,7 @@
         <v>2291.68</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>1451.52</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>6500</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>19303.1</v>
+        <v>23227.39</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2565,13 +2565,13 @@
         <v>4168.07156573679</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>442.27</v>
+        <v>2915.04</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>3725.80156573679</v>
+        <v>1253.03156573679</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.1061090226078736</v>
+        <v>0.6993737880997032</v>
       </c>
     </row>
     <row r="4">
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>15947.15</v>
+        <v>17398.67</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>28319.09</v>
+        <v>26867.57</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.3602553548708903</v>
+        <v>0.3930460323713963</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>19303.1</v>
+        <v>23227.39</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46074.89762291768</v>
+        <v>42150.60762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2952537658209566</v>
+        <v>0.3552783940243811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 12:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>6678.14</v>
+        <v>6978.81</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="2" t="n">
-        <v>0</v>
+        <v>2156.54</v>
       </c>
       <c r="N21" s="2" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>6 de 20</t>
+          <t>7 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2309,7 +2309,7 @@
         <v>45.91</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>6678.14</v>
+        <v>6978.81</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>8000</v>
@@ -2444,7 +2444,7 @@
         <v>1964.99</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>2156.54</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>5000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>23227.39</v>
+        <v>25684.6</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>17398.67</v>
+        <v>19855.88</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>26867.57</v>
+        <v>24410.36</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.3930460323713963</v>
+        <v>0.4485558294537779</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>23227.39</v>
+        <v>25684.6</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>42150.60762291768</v>
+        <v>39693.39762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.3552783940243811</v>
+        <v>0.3928630568978528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-09 12:35:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1730,10 +1730,10 @@
         <v>0</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>0</v>
+        <v>1593.9</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>0</v>
+        <v>658.8</v>
       </c>
       <c r="J21" s="2" t="n">
         <v>0</v>
@@ -1791,12 +1791,12 @@
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>1 de 20</t>
+          <t>2 de 20</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>1 de 20</t>
+          <t>2 de 20</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
@@ -2444,7 +2444,7 @@
         <v>1964.99</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>2156.54</v>
+        <v>4409.24</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>5000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>25684.6</v>
+        <v>27937.3</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2490,7 +2490,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2661,13 +2661,13 @@
         <v>2400</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>603</v>
+        <v>2196.9</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1797</v>
+        <v>203.0999999999999</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.25125</v>
+        <v>0.915375</v>
       </c>
     </row>
     <row r="8">
@@ -2685,13 +2685,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>28.8</v>
+        <v>687.6</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>596.2</v>
+        <v>-62.60000000000002</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.04608</v>
+        <v>1.10016</v>
       </c>
     </row>
     <row r="9">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>25684.6</v>
+        <v>27937.3</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>39693.39762291769</v>
+        <v>37440.69762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.3928630568978528</v>
+        <v>0.427319603165803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-18 11:05:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0</v>
+        <v>239.4</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>0</v>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>2 de 20</t>
+          <t>3 de 20</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
@@ -2147,7 +2147,7 @@
         <v>4711.21</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>3233.78</v>
+        <v>3473.18</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>6000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>27931.54</v>
+        <v>28170.94</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2490,7 +2490,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="24" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2685,13 +2685,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>687.6</v>
+        <v>927</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-62.60000000000002</v>
+        <v>-302</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>1.10016</v>
+        <v>1.4832</v>
       </c>
     </row>
     <row r="9">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>27931.54</v>
+        <v>28170.94</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>37446.45762291769</v>
+        <v>37207.05762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4272315001309988</v>
+        <v>0.4308932825150479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-18 11:10:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1070,7 +1070,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0</v>
+        <v>782.1</v>
       </c>
       <c r="I10" s="2" t="n">
         <v>239.4</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>3233.78</v>
+        <v>5283.42</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>6978.81</v>
+        <v>12316.05</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>2 de 20</t>
+          <t>3 de 20</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
@@ -1869,7 +1869,7 @@
     <col width="13" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2147,7 +2147,7 @@
         <v>4711.21</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>3473.18</v>
+        <v>6304.92</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>6000</v>
@@ -2309,7 +2309,7 @@
         <v>45.91</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>6978.81</v>
+        <v>12316.05</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>8000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>28170.94</v>
+        <v>36339.92</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2489,8 +2489,8 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2661,13 +2661,13 @@
         <v>2400</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>2196.9</v>
+        <v>2979</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>203.0999999999999</v>
+        <v>-579</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.915375</v>
+        <v>1.24125</v>
       </c>
     </row>
     <row r="8">
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>19850.12</v>
+        <v>27237</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>24416.12</v>
+        <v>17029.24</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.4484257077176648</v>
+        <v>0.6152996052974005</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>28170.94</v>
+        <v>36339.92</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>37207.05762291769</v>
+        <v>29038.07762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.4308932825150479</v>
+        <v>0.5558432702328797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-21 14:40:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1094,7 +1094,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="2" t="n">
-        <v>0</v>
+        <v>110.13</v>
       </c>
       <c r="Q10" s="2" t="n">
         <v>0</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="P22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="Q22" s="4" t="inlineStr">
@@ -2147,7 +2147,7 @@
         <v>4711.21</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>6304.92</v>
+        <v>6415.05</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>6000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>36339.92</v>
+        <v>36450.05</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2733,13 +2733,13 @@
         <v>650.25</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>110.13</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>650.25</v>
+        <v>540.12</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0</v>
+        <v>0.1693656286043829</v>
       </c>
     </row>
     <row r="11">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>36339.92</v>
+        <v>36450.05</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>29038.07762291769</v>
+        <v>28927.94762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5558432702328797</v>
+        <v>0.5575277819035369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-21 15:00:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -905,7 +905,7 @@
         <v>86.56999999999999</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>697.36</v>
+        <v>846.1900000000001</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>0</v>
@@ -2066,7 +2066,7 @@
         <v>177.41</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>2296.73</v>
+        <v>2445.56</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1500</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>36450.05</v>
+        <v>36598.88</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2489,7 +2489,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>27237</v>
+        <v>27385.83</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>17029.24</v>
+        <v>16880.41</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.6152996052974005</v>
+        <v>0.6186617611976983</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>36450.05</v>
+        <v>36598.88</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>28927.94762291769</v>
+        <v>28779.11762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5575277819035369</v>
+        <v>0.5598042358392847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 14:40:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>3969.29</v>
+        <v>4994.11</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
@@ -2012,7 +2012,7 @@
         <v>12.1</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>4371.1</v>
+        <v>5395.92</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>4000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>36598.88</v>
+        <v>37623.7</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>27385.83</v>
+        <v>28410.65</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>16880.41</v>
+        <v>15855.59</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.6186617611976983</v>
+        <v>0.6418130385594079</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>36598.88</v>
+        <v>37623.7</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>28779.11762291769</v>
+        <v>27754.29762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5598042358392847</v>
+        <v>0.5754795400281782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 14:50:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="2" t="n">
-        <v>0</v>
+        <v>2925.73</v>
       </c>
       <c r="N20" s="2" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="M22" s="4" t="inlineStr">
         <is>
-          <t>7 de 20</t>
+          <t>8 de 20</t>
         </is>
       </c>
       <c r="N22" s="4" t="inlineStr">
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0</v>
+        <v>2925.73</v>
       </c>
       <c r="G20" s="2" t="n">
         <v>500</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>37623.7</v>
+        <v>40549.43</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>28410.65</v>
+        <v>31336.38</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>15855.59</v>
+        <v>12929.86</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.6418130385594079</v>
+        <v>0.7079069738021572</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>37623.7</v>
+        <v>40549.43</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>27754.29762291769</v>
+        <v>24828.56762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.5754795400281782</v>
+        <v>0.6202305282256879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-07-24 14:55:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>4994.11</v>
+        <v>7043.75</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
@@ -2012,7 +2012,7 @@
         <v>12.1</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>5395.92</v>
+        <v>7445.56</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>4000</v>
@@ -2461,7 +2461,7 @@
         <v>16273.63</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>40549.43</v>
+        <v>42599.07</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>52500</v>
@@ -2877,13 +2877,13 @@
         <v>44266.24</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>31336.38</v>
+        <v>33386.02</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>12929.86</v>
+        <v>10880.22</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.7079069738021572</v>
+        <v>0.7542095285255761</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>65377.99762291768</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>40549.43</v>
+        <v>42599.06999999999</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>24828.56762291769</v>
+        <v>22778.92762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.6202305282256879</v>
+        <v>0.6515811366034751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-05 16:45:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -890,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0</v>
+        <v>68.73</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0</v>
+        <v>42.63</v>
       </c>
       <c r="J7" s="2" t="n">
         <v>0</v>
@@ -1791,12 +1791,12 @@
       </c>
       <c r="H22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="I22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="J22" s="4" t="inlineStr">
@@ -2066,7 +2066,7 @@
         <v>2898.45</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0</v>
+        <v>111.36</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1000</v>
@@ -2461,7 +2461,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>0</v>
+        <v>111.36</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>51500</v>
@@ -2661,13 +2661,13 @@
         <v>2400</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>68.73</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2400</v>
+        <v>2331.27</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0</v>
+        <v>0.0286375</v>
       </c>
     </row>
     <row r="8">
@@ -2685,13 +2685,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0</v>
+        <v>42.63</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>625</v>
+        <v>582.37</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0</v>
+        <v>0.068208</v>
       </c>
     </row>
     <row r="9">
@@ -2944,13 +2944,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>111.36</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>59388.22762291769</v>
+        <v>59276.86762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0</v>
+        <v>0.001875119101163858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 08:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0</v>
+        <v>129.6</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>0</v>
@@ -1766,7 +1766,7 @@
     <row r="22">
       <c r="C22" s="4" t="inlineStr">
         <is>
-          <t>0 de 20</t>
+          <t>1 de 20</t>
         </is>
       </c>
       <c r="D22" s="4" t="inlineStr">
@@ -2228,7 +2228,7 @@
         <v>5370.47</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>129.6</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>6500</v>
@@ -2461,7 +2461,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>2789.18</v>
+        <v>2918.78</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>51500</v>
@@ -2490,7 +2490,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2541,13 +2541,13 @@
         <v>782.465010521559</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0</v>
+        <v>129.6</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>782.465010521559</v>
+        <v>652.8650105215589</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>0</v>
+        <v>0.1656304093567251</v>
       </c>
     </row>
     <row r="3">
@@ -2944,13 +2944,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>2789.18</v>
+        <v>2918.78</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>56599.04762291769</v>
+        <v>56469.44762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.04696520020280361</v>
+        <v>0.04914745088088223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-08 15:50:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0</v>
+        <v>-21.92</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>0</v>
@@ -2066,7 +2066,7 @@
         <v>2898.45</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>111.36</v>
+        <v>89.44</v>
       </c>
       <c r="G7" s="2" t="n">
         <v>1000</v>
@@ -2461,7 +2461,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F22" s="6" t="n">
-        <v>2918.78</v>
+        <v>2896.86</v>
       </c>
       <c r="G22" s="6" t="n">
         <v>51500</v>
@@ -2489,7 +2489,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2877,13 +2877,13 @@
         <v>38776.47</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2677.82</v>
+        <v>2655.9</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>36098.65</v>
+        <v>36120.57</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.06905785905730975</v>
+        <v>0.06849256778659842</v>
       </c>
     </row>
     <row r="17">
@@ -2944,13 +2944,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>2918.78</v>
+        <v>2896.86</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>56469.44762291769</v>
+        <v>56491.36762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.04914745088088223</v>
+        <v>0.04877835416125659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-15 16:00:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
+          <t>FERRETERIAS FERRIGONZ SA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>1289.32</v>
+        <v>0</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
+          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>1289.32</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MEGAMAFERS S.A.</t>
+          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>1388.5</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2" t="n">
         <v>0</v>
@@ -1231,11 +1231,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
+          <t>MEGAMAFERS S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>129.6</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>0</v>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>1388.5</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1291,11 +1291,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ORTEGA PAREDES RUDHT ELENA</t>
+          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>129.6</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OÑATE PEREZ MERCY YOLANDA</t>
+          <t>ORTEGA PAREDES RUDHT ELENA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PADILLA MIER BERTHA MARIETA</t>
+          <t>OÑATE PEREZ MERCY YOLANDA</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PAVIMARSA S.A.</t>
+          <t>PADILLA MIER BERTHA MARIETA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SARZOSA UNDA JOSE DOMINGO</t>
+          <t>PAVIMARSA S.A.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
+          <t>SARZOSA UNDA JOSE DOMINGO</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1711,137 +1711,197 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>TULCAN NARVAEZ EDITH MARITZA</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="C22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="E22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="G22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="H22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
-      <c r="I22" s="4" t="inlineStr">
-        <is>
-          <t>1 de 20</t>
-        </is>
-      </c>
-      <c r="J22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="M22" s="4" t="inlineStr">
-        <is>
-          <t>2 de 20</t>
-        </is>
-      </c>
-      <c r="N22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="O22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="P22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="Q22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
-        </is>
-      </c>
-      <c r="R22" s="4" t="inlineStr">
-        <is>
-          <t>0 de 20</t>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="C23" s="4" t="inlineStr">
+        <is>
+          <t>1 de 21</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
+          <t>1 de 21</t>
+        </is>
+      </c>
+      <c r="I23" s="4" t="inlineStr">
+        <is>
+          <t>1 de 21</t>
+        </is>
+      </c>
+      <c r="J23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="K23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="L23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="M23" s="4" t="inlineStr">
+        <is>
+          <t>2 de 21</t>
+        </is>
+      </c>
+      <c r="N23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="O23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="P23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="Q23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="R23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1916,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2134,23 +2194,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
+          <t>FERRETERIAS FERRIGONZ SA</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>11565.71</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>4711.21</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>12314.93</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>1289.32</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2161,23 +2221,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
+          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0</v>
+        <v>11565.71</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>4711.21</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0</v>
+        <v>12314.93</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>1289.32</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="12">
@@ -2188,23 +2248,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MEGAMAFERS S.A.</t>
+          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>1565.15</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>4381.39</v>
+        <v>0</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>3399.19</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>1388.5</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2215,23 +2275,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
+          <t>MEGAMAFERS S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>9034.549999999999</v>
+        <v>1565.15</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>2291.68</v>
+        <v>4381.39</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>5370.47</v>
+        <v>3399.19</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>129.6</v>
+        <v>1388.5</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>6500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="14">
@@ -2242,23 +2302,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ORTEGA PAREDES RUDHT ELENA</t>
+          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>0</v>
+        <v>9034.549999999999</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>0</v>
+        <v>2291.68</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>0</v>
+        <v>5370.47</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>129.6</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>500</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="15">
@@ -2269,17 +2329,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OÑATE PEREZ MERCY YOLANDA</t>
+          <t>ORTEGA PAREDES RUDHT ELENA</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>288.17</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>431.64</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1319.85</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
@@ -2296,23 +2356,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>PADILLA MIER BERTHA MARIETA</t>
+          <t>OÑATE PEREZ MERCY YOLANDA</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>0</v>
+        <v>288.17</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>45.91</v>
+        <v>431.64</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>12316.05</v>
+        <v>1319.85</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>8000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17">
@@ -2323,23 +2383,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PAVIMARSA S.A.</t>
+          <t>PADILLA MIER BERTHA MARIETA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0</v>
+        <v>45.91</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0</v>
+        <v>12316.05</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="18">
@@ -2350,23 +2410,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SARZOSA UNDA JOSE DOMINGO</t>
+          <t>PAVIMARSA S.A.</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>290.56</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>1935.16</v>
+        <v>0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>1702.17</v>
+        <v>0</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>4500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -2377,23 +2437,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
+          <t>SARZOSA UNDA JOSE DOMINGO</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>0</v>
+        <v>290.56</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0</v>
+        <v>1935.16</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0</v>
+        <v>1702.17</v>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>0</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="20">
@@ -2404,7 +2464,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -2414,13 +2474,13 @@
         <v>0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>2925.73</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>1500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2431,39 +2491,66 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>2925.73</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>TULCAN NARVAEZ EDITH MARITZA</t>
         </is>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C22" s="2" t="n">
         <v>15564.83</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D22" s="2" t="n">
         <v>1964.99</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E22" s="2" t="n">
         <v>5388.82</v>
       </c>
-      <c r="F21" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2" t="n">
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
         <v>5000</v>
       </c>
     </row>
-    <row r="22">
-      <c r="C22" s="6" t="n">
+    <row r="23">
+      <c r="C23" s="6" t="n">
         <v>54669.1</v>
       </c>
-      <c r="D22" s="6" t="n">
+      <c r="D23" s="6" t="n">
         <v>16273.63</v>
       </c>
-      <c r="E22" s="6" t="n">
+      <c r="E23" s="6" t="n">
         <v>66172.89999999999</v>
       </c>
-      <c r="F22" s="6" t="n">
+      <c r="F23" s="6" t="n">
         <v>2896.86</v>
       </c>
-      <c r="G22" s="6" t="n">
+      <c r="G23" s="6" t="n">
         <v>51500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-08-19 12:20:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>1388.5</v>
+        <v>5034.91</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -2288,7 +2288,7 @@
         <v>3399.19</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1388.5</v>
+        <v>5034.91</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>2909.72</v>
+        <v>6556.13</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>
@@ -2578,7 +2578,7 @@
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2964,13 +2964,13 @@
         <v>38776.47</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2668.76</v>
+        <v>6315.17</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>36107.71</v>
+        <v>32461.3</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.06882421220910516</v>
+        <v>0.1628608792909721</v>
       </c>
     </row>
     <row r="17">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>2909.72</v>
+        <v>6556.13</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>56478.50762291768</v>
+        <v>52832.09762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.04899489539366469</v>
+        <v>0.1103944377937626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 11:40:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0</v>
+        <v>60.78</v>
       </c>
       <c r="N10" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>3 de 21</t>
+          <t>4 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>60.78</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2548,7 +2548,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>7471.97</v>
+        <v>7532.75</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>
@@ -2964,13 +2964,13 @@
         <v>38776.47</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>6315.17</v>
+        <v>6375.95</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>32461.3</v>
+        <v>32400.52</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1628608792909721</v>
+        <v>0.1644283247030996</v>
       </c>
     </row>
     <row r="17">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>7471.97</v>
+        <v>7532.75</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51916.25762291768</v>
+        <v>51855.47762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1258156759188516</v>
+        <v>0.1268391110748208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 17:15:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1133,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0</v>
+        <v>813.11</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>0</v>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>5034.91</v>
+        <v>8423.42</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="I23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="J23" s="4" t="inlineStr">
@@ -2234,7 +2234,7 @@
         <v>12314.93</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1289.32</v>
+        <v>2102.43</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>6000</v>
@@ -2288,7 +2288,7 @@
         <v>3399.19</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>5034.91</v>
+        <v>8423.42</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>7532.75</v>
+        <v>11734.37</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>
@@ -2772,13 +2772,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>42.63</v>
+        <v>855.74</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>582.37</v>
+        <v>-230.74</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>0.068208</v>
+        <v>1.369184</v>
       </c>
     </row>
     <row r="9">
@@ -2964,13 +2964,13 @@
         <v>38776.47</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>6375.95</v>
+        <v>9764.459999999999</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>32400.52</v>
+        <v>29012.01</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.1644283247030996</v>
+        <v>0.2518140511500918</v>
       </c>
     </row>
     <row r="17">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>7532.75</v>
+        <v>11734.37</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>51855.47762291769</v>
+        <v>47653.85762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.1268391110748208</v>
+        <v>0.197587475997882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-27 17:20:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1130,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0</v>
+        <v>1018.8</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>813.11</v>
+        <v>1007.51</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>0</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
@@ -2234,7 +2234,7 @@
         <v>12314.93</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>2102.43</v>
+        <v>3315.63</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>6000</v>
@@ -2548,7 +2548,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>11734.37</v>
+        <v>12947.57</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>
@@ -2577,7 +2577,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2748,13 +2748,13 @@
         <v>2400</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>68.73</v>
+        <v>1087.53</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>2331.27</v>
+        <v>1312.47</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.0286375</v>
+        <v>0.4531375</v>
       </c>
     </row>
     <row r="8">
@@ -2772,13 +2772,13 @@
         <v>625</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>855.74</v>
+        <v>1050.14</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>-230.74</v>
+        <v>-425.1400000000001</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>1.369184</v>
+        <v>1.680224</v>
       </c>
     </row>
     <row r="9">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>11734.37</v>
+        <v>12947.57</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>47653.85762291768</v>
+        <v>46440.65762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.197587475997882</v>
+        <v>0.2180157670676736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-28 08:30:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -2576,7 +2576,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2964,13 +2964,13 @@
         <v>38776.47</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>9764.459999999999</v>
+        <v>11479.77</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>29012.01</v>
+        <v>27296.7</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2518140511500918</v>
+        <v>0.2960498983017278</v>
       </c>
     </row>
     <row r="17">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>12947.57</v>
+        <v>14662.88</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>46440.65762291769</v>
+        <v>44725.34762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2180157670676736</v>
+        <v>0.2468987640631601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-28 15:05:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0</v>
+        <v>147.81</v>
       </c>
       <c r="M11" s="2" t="n">
         <v>1289.32</v>
@@ -1742,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="L21" s="2" t="n">
-        <v>0</v>
+        <v>873.8</v>
       </c>
       <c r="M21" s="2" t="n">
         <v>0</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -2234,7 +2234,7 @@
         <v>12314.93</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>3315.63</v>
+        <v>3463.44</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>6000</v>
@@ -2504,7 +2504,7 @@
         <v>2925.73</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0</v>
+        <v>873.8</v>
       </c>
       <c r="G21" s="2" t="n">
         <v>1500</v>
@@ -2548,7 +2548,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>12947.57</v>
+        <v>13969.18</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>
@@ -2940,13 +2940,13 @@
         <v>7465</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>1021.61</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>7465</v>
+        <v>6443.39</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0</v>
+        <v>0.1368533154722036</v>
       </c>
     </row>
     <row r="16">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>14662.88</v>
+        <v>15684.49</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>44725.34762291769</v>
+        <v>43703.73762291769</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2468987640631601</v>
+        <v>0.2641009948905668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-08-28 16:45:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>0</v>
+        <v>-2156.54</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -1929,7 +1929,7 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2531,7 +2531,7 @@
         <v>5388.82</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
+        <v>-2156.54</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>66172.89999999999</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>13969.18</v>
+        <v>11812.64</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>
@@ -2576,7 +2576,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2964,13 +2964,13 @@
         <v>38776.47</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>11479.77</v>
+        <v>9323.23</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>27296.7</v>
+        <v>29453.24</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>0.2960498983017278</v>
+        <v>0.2404352433318453</v>
       </c>
     </row>
     <row r="17">
@@ -3031,13 +3031,13 @@
         <v>59388.22762291769</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>15684.49</v>
+        <v>13527.95</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>43703.73762291769</v>
+        <v>45860.27762291768</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>0.2641009948905668</v>
+        <v>0.2277884109607544</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-02 09:50:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>0</v>
+        <v>3568.07</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2531,7 +2531,7 @@
         <v>-2156.54</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
+        <v>3568.07</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>916.2</v>
+        <v>4484.27</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-02 09:55:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0</v>
+        <v>3910.61</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2315,7 +2315,7 @@
         <v>142.46</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>3910.61</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>6500</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>4484.27</v>
+        <v>8394.880000000001</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-02 10:50:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>3568.07</v>
+        <v>4763.94</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -2531,7 +2531,7 @@
         <v>-2156.54</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>3568.07</v>
+        <v>4763.94</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>8394.880000000001</v>
+        <v>9590.75</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-02 11:00:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0</v>
+        <v>475.2</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>4763.94</v>
+        <v>6879.73</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="E23" s="4" t="inlineStr">
@@ -2531,7 +2531,7 @@
         <v>-2156.54</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>4763.94</v>
+        <v>7354.93</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>9590.75</v>
+        <v>12181.74</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>51500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-09 13:25:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>4018.52</v>
+        <v>3981.45</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -2234,7 +2234,7 @@
         <v>3463.44</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>4934.72</v>
+        <v>4897.65</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>7000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>24239.83</v>
+        <v>24202.76</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2868,13 +2868,13 @@
         <v>36823.6430921171</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>21833.23</v>
+        <v>21796.16</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>14990.4130921171</v>
+        <v>15027.4830921171</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5929133612712502</v>
+        <v>0.5919066710883352</v>
       </c>
     </row>
     <row r="13">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>24239.83</v>
+        <v>24202.76</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>31184.91316613378</v>
+        <v>31221.98316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.437346726665777</v>
+        <v>0.4366778918118402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 17:15:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1790,10 +1790,10 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0</v>
+        <v>-67.65000000000001</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>0</v>
+        <v>-57.6</v>
       </c>
       <c r="J22" s="2" t="n">
         <v>0</v>
@@ -2531,7 +2531,7 @@
         <v>-2156.54</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>7354.93</v>
+        <v>7229.68</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>6000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>24202.76</v>
+        <v>24077.51</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2577,7 +2577,7 @@
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="23" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2724,13 +2724,13 @@
         <v>2907.58368146026</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1803.6</v>
+        <v>1735.95</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1103.98368146026</v>
+        <v>1171.63368146026</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.6203088879265507</v>
+        <v>0.5970421457064181</v>
       </c>
     </row>
     <row r="7">
@@ -2748,13 +2748,13 @@
         <v>886.711016287574</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>127.8</v>
+        <v>70.2</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>758.9110162875741</v>
+        <v>816.511016287574</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.1441281292918464</v>
+        <v>0.07916897242791564</v>
       </c>
     </row>
     <row r="8">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>24202.76</v>
+        <v>24077.51</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>31221.98316613378</v>
+        <v>31347.23316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.4366778918118402</v>
+        <v>0.4344180707852535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-10 17:20:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>-67.65000000000001</v>
+        <v>-255.75</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>-57.6</v>
@@ -2531,7 +2531,7 @@
         <v>-2156.54</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>7229.68</v>
+        <v>7041.58</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>6000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>24077.51</v>
+        <v>23889.41</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2724,13 +2724,13 @@
         <v>2907.58368146026</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1735.95</v>
+        <v>1547.85</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1171.63368146026</v>
+        <v>1359.73368146026</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.5970421457064181</v>
+        <v>0.5323492527040982</v>
       </c>
     </row>
     <row r="7">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>24077.51</v>
+        <v>23889.41</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>31347.23316613378</v>
+        <v>31535.33316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.4344180707852535</v>
+        <v>0.431024279686643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 14:25:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>3910.61</v>
+        <v>5583.28</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -2315,7 +2315,7 @@
         <v>142.46</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>3910.61</v>
+        <v>5583.28</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>7000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>23999.03</v>
+        <v>25671.7</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2868,13 +2868,13 @@
         <v>36823.6430921171</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>21905.78</v>
+        <v>23578.45</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>14917.8630921171</v>
+        <v>13245.1930921171</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5948835628566421</v>
+        <v>0.64030736831271</v>
       </c>
     </row>
     <row r="13">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>23999.03</v>
+        <v>25671.7</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>31425.71316613378</v>
+        <v>29753.04316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.4330020967000916</v>
+        <v>0.4631812171515158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 14:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>5583.28</v>
+        <v>11342.53</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -2315,7 +2315,7 @@
         <v>142.46</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>5583.28</v>
+        <v>11342.53</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>7000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>25671.7</v>
+        <v>31430.95</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2576,8 +2576,8 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2868,13 +2868,13 @@
         <v>36823.6430921171</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>23578.45</v>
+        <v>29337.7</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>13245.1930921171</v>
+        <v>7485.943092117097</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.64030736831271</v>
+        <v>0.7967082433047037</v>
       </c>
     </row>
     <row r="13">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>25671.7</v>
+        <v>31430.95</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>29753.04316613378</v>
+        <v>23993.79316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.4631812171515158</v>
+        <v>0.5670923887872029</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-11 14:35:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0</v>
+        <v>1392.03</v>
       </c>
       <c r="M6" s="2" t="n">
         <v>0</v>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
@@ -2099,7 +2099,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0</v>
+        <v>1392.03</v>
       </c>
       <c r="G6" s="2" t="n">
         <v>4000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>31430.95</v>
+        <v>32822.98</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2844,13 +2844,13 @@
         <v>5844.44916370549</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>1392.03</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>5844.44916370549</v>
+        <v>4452.41916370549</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0</v>
+        <v>0.2381798456977983</v>
       </c>
     </row>
     <row r="12">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>31430.95</v>
+        <v>32822.98</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>23993.79316613378</v>
+        <v>22601.76316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.5670923887872029</v>
+        <v>0.592208066740413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-12 12:50:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>2635.78</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>6 de 21</t>
+          <t>7 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2288,7 +2288,7 @@
         <v>8423.42</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>2635.78</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>32822.98</v>
+        <v>35458.76</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2576,7 +2576,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="23" customWidth="1" min="5" max="5"/>
     <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2868,13 +2868,13 @@
         <v>36823.6430921171</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>29337.7</v>
+        <v>31973.48</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>7485.943092117097</v>
+        <v>4850.163092117098</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.7967082433047037</v>
+        <v>0.8682867124259256</v>
       </c>
     </row>
     <row r="13">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>32822.98</v>
+        <v>35458.76</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>22601.76316613378</v>
+        <v>19965.98316613378</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.592208066740413</v>
+        <v>0.6397640832310865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-24 08:40:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>443.14</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>4500</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>44864.53</v>
+        <v>45307.67</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>

</xml_diff>

<commit_message>
Actualización automática 2025-09-26 11:50:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>4473.94</v>
+        <v>10280.02</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -2288,7 +2288,7 @@
         <v>8423.42</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>5833.17</v>
+        <v>11639.25</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>45307.67</v>
+        <v>51113.75</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2868,13 +2868,13 @@
         <v>36823.6430921171</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>38098.83</v>
+        <v>43904.91</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-1275.186907882904</v>
+        <v>-7081.266907882906</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>1.034629569504922</v>
+        <v>1.192302181784909</v>
       </c>
     </row>
     <row r="13">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44864.53</v>
+        <v>50670.61</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>10560.21316613377</v>
+        <v>4754.13316613377</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.8094675308737129</v>
+        <v>0.9142236319998196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-09-26 14:45:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>10280.02</v>
+        <v>11932.44</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -2288,7 +2288,7 @@
         <v>8423.42</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>11639.25</v>
+        <v>13291.67</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>11812.64</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>51113.75</v>
+        <v>52766.17</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>53000</v>
@@ -2868,13 +2868,13 @@
         <v>36823.6430921171</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>43904.91</v>
+        <v>45557.33</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>-7081.266907882906</v>
+        <v>-8733.686907882904</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>1.192302181784909</v>
+        <v>1.237176068810871</v>
       </c>
     </row>
     <row r="13">
@@ -2935,13 +2935,13 @@
         <v>55424.74316613378</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>50670.61</v>
+        <v>52323.03</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>4754.13316613377</v>
+        <v>3101.713166133772</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>0.9142236319998196</v>
+        <v>0.9440373921655082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-13 16:30:10
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -2021,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4">
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="6">
@@ -2102,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="7">
@@ -2129,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8">
@@ -2156,7 +2156,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="9">
@@ -2237,7 +2237,7 @@
         <v>95.04000000000001</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="12">
@@ -2291,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="14">
@@ -2318,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>0</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="15">
@@ -2345,7 +2345,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16">
@@ -2372,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="17">
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>0</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="18">
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="21">
@@ -2507,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="22">
@@ -2534,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>0</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="23">
@@ -2551,7 +2551,7 @@
         <v>95.04000000000001</v>
       </c>
       <c r="G23" s="6" t="n">
-        <v>0</v>
+        <v>52500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-16 14:30:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>95.04000000000001</v>
+        <v>552.96</v>
       </c>
       <c r="E11" s="2" t="n">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>4524.27</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2234,7 +2234,7 @@
         <v>6897.82</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>95.04000000000001</v>
+        <v>5077.23</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>7000</v>
@@ -2548,7 +2548,7 @@
         <v>61624.43</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>95.04000000000001</v>
+        <v>5077.23</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2576,9 +2576,9 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="11" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="22" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2652,13 +2652,13 @@
         <v>5504.61890386263</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>95.04000000000001</v>
+        <v>552.96</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>5409.57890386263</v>
+        <v>4951.65890386263</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.01726550042062127</v>
+        <v>0.1004538206290692</v>
       </c>
     </row>
     <row r="4">
@@ -2868,13 +2868,13 @@
         <v>37739.74</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>4524.27</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>37739.74</v>
+        <v>33215.47</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0</v>
+        <v>0.1198807940913213</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55424.74147880389</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>95.04000000000001</v>
+        <v>5077.23</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>55329.70147880389</v>
+        <v>50347.51147880389</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.001714757659922441</v>
+        <v>0.09160584000092609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-16 17:30:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0</v>
+        <v>23.76</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2072,7 +2072,7 @@
         <v>5180.39</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0</v>
+        <v>23.76</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>3000</v>
@@ -2548,7 +2548,7 @@
         <v>61624.43</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>5077.23</v>
+        <v>5100.99</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2868,13 +2868,13 @@
         <v>37739.74</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>4524.27</v>
+        <v>4548.03</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>33215.47</v>
+        <v>33191.71</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.1198807940913213</v>
+        <v>0.1205103691758343</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55424.74147880389</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>5077.23</v>
+        <v>5100.99</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>50347.51147880389</v>
+        <v>50323.7514788039</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.09160584000092609</v>
+        <v>0.09203452941590669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-25 10:30:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>0</v>
+        <v>9155.459999999999</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>0</v>
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0</v>
+        <v>1526.4</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0</v>
+        <v>1940.3</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
@@ -1802,7 +1802,7 @@
         <v>0</v>
       </c>
       <c r="L22" s="2" t="n">
-        <v>0</v>
+        <v>1611.96</v>
       </c>
       <c r="M22" s="2" t="n">
         <v>0</v>
@@ -1831,52 +1831,52 @@
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
+          <t>2 de 21</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="G23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
           <t>1 de 21</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr">
+      <c r="I23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
+      <c r="J23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="G23" s="4" t="inlineStr">
+      <c r="K23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="H23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="I23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="J23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>2 de 21</t>
+          <t>3 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2396,7 +2396,7 @@
         <v>6213.78</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0</v>
+        <v>9155.459999999999</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>9500</v>
@@ -2531,7 +2531,7 @@
         <v>10848.32</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
+        <v>5078.66</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>6000</v>
@@ -2548,7 +2548,7 @@
         <v>61624.43</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>3519.52</v>
+        <v>17753.64</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2576,8 +2576,8 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2652,13 +2652,13 @@
         <v>5504.61890386263</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>552.96</v>
+        <v>2079.36</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>4951.65890386263</v>
+        <v>3425.25890386263</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>0.1004538206290692</v>
+        <v>0.3777482213238956</v>
       </c>
     </row>
     <row r="4">
@@ -2724,13 +2724,13 @@
         <v>2907.58368146026</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>1940.3</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>2907.58368146026</v>
+        <v>967.2836814602599</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>0.6673238718362643</v>
       </c>
     </row>
     <row r="7">
@@ -2844,13 +2844,13 @@
         <v>5844.44916370549</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0</v>
+        <v>1611.96</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>5844.44916370549</v>
+        <v>4232.48916370549</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0</v>
+        <v>0.2758104236769487</v>
       </c>
     </row>
     <row r="12">
@@ -2868,13 +2868,13 @@
         <v>37739.74</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>2966.56</v>
+        <v>12122.02</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>34773.18</v>
+        <v>25617.72</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.078605734962668</v>
+        <v>0.3212004110256192</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55424.74147880389</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>3519.52</v>
+        <v>17753.64</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>51905.2214788039</v>
+        <v>37671.1014788039</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.06350088256786857</v>
+        <v>0.3203197620107896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-10-31 08:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0</v>
+        <v>507.6</v>
       </c>
       <c r="L10" s="2" t="n">
         <v>0</v>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0</v>
+        <v>4850.15</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>0</v>
+        <v>970.08</v>
       </c>
       <c r="I16" s="2" t="n">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="2" t="n">
-        <v>0</v>
+        <v>2186.02</v>
       </c>
       <c r="N16" s="2" t="n">
         <v>0</v>
@@ -1505,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="2" t="n">
-        <v>9155.459999999999</v>
+        <v>16276.37</v>
       </c>
       <c r="N17" s="2" t="n">
         <v>0</v>
@@ -1851,24 +1851,24 @@
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
+          <t>2 de 21</t>
+        </is>
+      </c>
+      <c r="I23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="J23" s="4" t="inlineStr">
+        <is>
+          <t>0 de 21</t>
+        </is>
+      </c>
+      <c r="K23" s="4" t="inlineStr">
+        <is>
           <t>1 de 21</t>
         </is>
       </c>
-      <c r="I23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="J23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
           <t>2 de 21</t>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>3 de 21</t>
+          <t>5 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -1929,7 +1929,7 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
@@ -2207,7 +2207,7 @@
         <v>2272.64</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0</v>
+        <v>507.6</v>
       </c>
       <c r="G10" s="2" t="n">
         <v>0</v>
@@ -2315,7 +2315,7 @@
         <v>11342.53</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>4850.15</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>7000</v>
@@ -2369,7 +2369,7 @@
         <v>2350.99</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>0</v>
+        <v>3156.1</v>
       </c>
       <c r="G16" s="2" t="n">
         <v>500</v>
@@ -2396,7 +2396,7 @@
         <v>6213.78</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>9155.459999999999</v>
+        <v>16276.37</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>9500</v>
@@ -2548,7 +2548,7 @@
         <v>61624.43</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>27491.2</v>
+        <v>43125.96</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2576,8 +2576,8 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="23" customWidth="1" min="5" max="5"/>
     <col width="24" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
@@ -2724,13 +2724,13 @@
         <v>2907.58368146026</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>1858.63</v>
+        <v>2828.71</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>1048.95368146026</v>
+        <v>78.87368146025983</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.6392352563577983</v>
+        <v>0.972873117302458</v>
       </c>
     </row>
     <row r="7">
@@ -2820,13 +2820,13 @@
         <v>388.107983534392</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0</v>
+        <v>507.6</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>388.107983534392</v>
+        <v>-119.492016465608</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>0</v>
+        <v>1.307883428156843</v>
       </c>
     </row>
     <row r="11">
@@ -2868,13 +2868,13 @@
         <v>37739.74</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>21602.52</v>
+        <v>35759.6</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>16137.22</v>
+        <v>1980.139999999999</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5724077590359659</v>
+        <v>0.9475317000064124</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55424.74147880389</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>27491.2</v>
+        <v>43125.96</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>27933.5414788039</v>
+        <v>12298.78147880389</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.496009530518306</v>
+        <v>0.7780994344645284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-05 15:30:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0</v>
+        <v>3104.01</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2234,7 +2234,7 @@
         <v>5172.27</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0</v>
+        <v>3104.01</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>7000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>0</v>
+        <v>3104.01</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-11-07 16:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0</v>
+        <v>1742.32</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2288,7 +2288,7 @@
         <v>-494.21</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>0</v>
+        <v>1742.32</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>1799.97</v>
+        <v>3542.29</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-11-12 10:30:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>1742.32</v>
+        <v>4299.98</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -2288,7 +2288,7 @@
         <v>-494.21</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1742.32</v>
+        <v>4299.98</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>4066.3</v>
+        <v>6623.96</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2868,13 +2868,13 @@
         <v>44418</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>3703.25</v>
+        <v>6260.91</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>40714.75</v>
+        <v>38157.09</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.08337273177540637</v>
+        <v>0.1409543428339862</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55399.47101170094</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>4066.3</v>
+        <v>6623.96</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>51333.17101170094</v>
+        <v>48775.51101170094</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.07339961782561345</v>
+        <v>0.1195672066724419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-12 11:30:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>4299.98</v>
+        <v>4857.52</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -2288,7 +2288,7 @@
         <v>-494.21</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>4299.98</v>
+        <v>4857.52</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>6623.96</v>
+        <v>7181.500000000001</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2868,13 +2868,13 @@
         <v>44418</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>6260.91</v>
+        <v>6818.45</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>38157.09</v>
+        <v>37599.55</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.1409543428339862</v>
+        <v>0.1535064613445</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55399.47101170094</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>6623.96</v>
+        <v>7181.5</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>48775.51101170094</v>
+        <v>48217.97101170095</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.1195672066724419</v>
+        <v>0.12963120168572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-24 12:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0</v>
+        <v>2735.25</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>-1151.4</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>-185.33</v>
+        <v>12050.73</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -1851,19 +1851,19 @@
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
+          <t>1 de 21</t>
+        </is>
+      </c>
+      <c r="I23" s="4" t="inlineStr">
+        <is>
+          <t>2 de 21</t>
+        </is>
+      </c>
+      <c r="J23" s="4" t="inlineStr">
+        <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="I23" s="4" t="inlineStr">
-        <is>
-          <t>2 de 21</t>
-        </is>
-      </c>
-      <c r="J23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
       <c r="K23" s="4" t="inlineStr">
         <is>
           <t>1 de 21</t>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>3 de 21</t>
+          <t>4 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2531,7 +2531,7 @@
         <v>4205.02</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>-1489.37</v>
+        <v>13481.94</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>6000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>21283.68</v>
+        <v>36254.99</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2576,7 +2576,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2724,13 +2724,13 @@
         <v>2907.58368146026</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0</v>
+        <v>2735.25</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>2907.58368146026</v>
+        <v>172.3336814602599</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0</v>
+        <v>0.9407295884348513</v>
       </c>
     </row>
     <row r="7">
@@ -2868,13 +2868,13 @@
         <v>44418</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>10824.3</v>
+        <v>23060.36</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>33593.7</v>
+        <v>21357.64</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.2436917465892206</v>
+        <v>0.5191670043675988</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55399.47101170094</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>21283.68</v>
+        <v>36254.99000000001</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>34115.79101170094</v>
+        <v>19144.48101170094</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.3841856178645581</v>
+        <v>0.6544284509926562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-25 15:30:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1130,10 +1130,10 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0</v>
+        <v>769.02</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>384.5</v>
+        <v>566.3</v>
       </c>
       <c r="J11" s="2" t="n">
         <v>0</v>
@@ -1145,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>5809.48</v>
+        <v>8613.280000000001</v>
       </c>
       <c r="N11" s="2" t="n">
         <v>0</v>
@@ -1265,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>6343.23</v>
+        <v>11168.17</v>
       </c>
       <c r="N13" s="2" t="n">
         <v>0</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="H23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="I23" s="4" t="inlineStr">
@@ -2234,7 +2234,7 @@
         <v>5172.27</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>6193.98</v>
+        <v>9948.6</v>
       </c>
       <c r="G11" s="2" t="n">
         <v>7000</v>
@@ -2288,7 +2288,7 @@
         <v>-494.21</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>6343.23</v>
+        <v>11168.17</v>
       </c>
       <c r="G13" s="2" t="n">
         <v>5000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>36254.99</v>
+        <v>44834.55</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2576,7 +2576,7 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
     <col width="26" customWidth="1" min="6" max="6"/>
   </cols>
@@ -2724,13 +2724,13 @@
         <v>2907.58368146026</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2735.25</v>
+        <v>3504.27</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>172.3336814602599</v>
+        <v>-596.6863185397401</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>0.9407295884348513</v>
+        <v>1.205217247002869</v>
       </c>
     </row>
     <row r="7">
@@ -2748,13 +2748,13 @@
         <v>383.4</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>428.6</v>
+        <v>610.4</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>-45.20000000000005</v>
+        <v>-227</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>1.117892540427752</v>
+        <v>1.59207094418362</v>
       </c>
     </row>
     <row r="8">
@@ -2868,13 +2868,13 @@
         <v>44418</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>23060.36</v>
+        <v>30689.1</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>21357.64</v>
+        <v>13728.9</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.5191670043675988</v>
+        <v>0.6909158449277319</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55399.47101170094</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>36254.99000000001</v>
+        <v>44834.55</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>19144.48101170094</v>
+        <v>10564.92101170094</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.6544284509926562</v>
+        <v>0.8092956337169805</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-11-26 08:30:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>146.53</v>
+        <v>732.67</v>
       </c>
       <c r="E5" s="2" t="n">
         <v>0</v>
@@ -782,10 +782,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0</v>
+        <v>71.44</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>-1800.8</v>
+        <v>2259.14</v>
       </c>
       <c r="N5" s="2" t="n">
         <v>0</v>
@@ -1871,12 +1871,12 @@
       </c>
       <c r="L23" s="4" t="inlineStr">
         <is>
-          <t>1 de 21</t>
+          <t>2 de 21</t>
         </is>
       </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>4 de 21</t>
+          <t>5 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2072,7 +2072,7 @@
         <v>9421.780000000001</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>-1654.27</v>
+        <v>3063.25</v>
       </c>
       <c r="G5" s="2" t="n">
         <v>3000</v>
@@ -2548,7 +2548,7 @@
         <v>50808.59</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>44834.55</v>
+        <v>49552.07</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>
@@ -2576,9 +2576,9 @@
     <col width="31" customWidth="1" min="1" max="1"/>
     <col width="22" customWidth="1" min="2" max="2"/>
     <col width="22" customWidth="1" min="3" max="3"/>
-    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="24" customWidth="1" min="5" max="5"/>
-    <col width="26" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2652,13 +2652,13 @@
         <v>2564</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>9326.83</v>
+        <v>9912.969999999999</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>-6762.83</v>
+        <v>-7348.969999999999</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>3.637609204368175</v>
+        <v>3.866212948517941</v>
       </c>
     </row>
     <row r="4">
@@ -2844,13 +2844,13 @@
         <v>2678</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>13.67</v>
+        <v>85.11</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>2664.33</v>
+        <v>2592.89</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>0.005104555638536221</v>
+        <v>0.03178117998506348</v>
       </c>
     </row>
     <row r="12">
@@ -2868,13 +2868,13 @@
         <v>44418</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>30689.1</v>
+        <v>34749.04</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>13728.9</v>
+        <v>9668.959999999999</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>0.6909158449277319</v>
+        <v>0.7823188797334414</v>
       </c>
     </row>
     <row r="13">
@@ -2911,13 +2911,13 @@
         <v>55399.47101170094</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>44834.55</v>
+        <v>49552.07</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>10564.92101170094</v>
+        <v>5847.401011700942</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>0.8092956337169805</v>
+        <v>0.8944502374315829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización automática 2025-12-01 16:30:09
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1778,7 +1778,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0</v>
+        <v>457.92</v>
       </c>
       <c r="E22" s="2" t="n">
         <v>0</v>
@@ -1790,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>0</v>
+        <v>2847.34</v>
       </c>
       <c r="I22" s="2" t="n">
         <v>0</v>
@@ -1805,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="2" t="n">
-        <v>0</v>
+        <v>5082.56</v>
       </c>
       <c r="N22" s="2" t="n">
         <v>0</v>
@@ -1831,52 +1831,52 @@
       </c>
       <c r="D23" s="4" t="inlineStr">
         <is>
+          <t>1 de 21</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr">
+      <c r="F23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
+      <c r="G23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="G23" s="4" t="inlineStr">
+      <c r="H23" s="4" t="inlineStr">
+        <is>
+          <t>1 de 21</t>
+        </is>
+      </c>
+      <c r="I23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="H23" s="4" t="inlineStr">
+      <c r="J23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="I23" s="4" t="inlineStr">
+      <c r="K23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="J23" s="4" t="inlineStr">
+      <c r="L23" s="4" t="inlineStr">
         <is>
           <t>0 de 21</t>
         </is>
       </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="L23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
       <c r="M23" s="4" t="inlineStr">
         <is>
-          <t>0 de 21</t>
+          <t>1 de 21</t>
         </is>
       </c>
       <c r="N23" s="4" t="inlineStr">
@@ -2531,7 +2531,7 @@
         <v>13320.25</v>
       </c>
       <c r="F22" s="2" t="n">
-        <v>0</v>
+        <v>8387.82</v>
       </c>
       <c r="G22" s="2" t="n">
         <v>6000</v>
@@ -2548,7 +2548,7 @@
         <v>66667.3</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>0</v>
+        <v>8387.82</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-12-03 11:30:08
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>0</v>
+        <v>-1220.11</v>
       </c>
       <c r="R19" s="2" t="n">
         <v>0</v>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>0</v>
+        <v>-1220.11</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>0</v>
@@ -2548,7 +2548,7 @@
         <v>66667.3</v>
       </c>
       <c r="F23" s="6" t="n">
-        <v>8387.82</v>
+        <v>7167.71</v>
       </c>
       <c r="G23" s="6" t="n">
         <v>52500</v>

</xml_diff>

<commit_message>
Actualización automática 2025-12-05 14:30:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CHASIQUIZA CAMPAÑA JOSE LUIS</t>
+          <t>CARRION CARRION STEPHANIE DAYANA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -871,7 +871,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHONTASI SIMBAÑA SILVIA JANETH</t>
+          <t>CHASIQUIZA CAMPAÑA JOSE LUIS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
@@ -905,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>150.71</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2" t="n">
         <v>0</v>
@@ -931,7 +931,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DECORHOME S.C.C.</t>
+          <t>CHONTASI SIMBAÑA SILVIA JANETH</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
@@ -965,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0</v>
+        <v>150.71</v>
       </c>
       <c r="N8" s="2" t="n">
         <v>0</v>
@@ -991,7 +991,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ESCUDERO CRUZ SILVIA RAQUEL</t>
+          <t>DECORHOME S.C.C.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FERRETERIAS FERRIGONZ SA</t>
+          <t>ESCUDERO CRUZ SILVIA RAQUEL</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
+          <t>FERRETERIAS FERRIGONZ SA</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>1996.4</v>
+        <v>0</v>
       </c>
       <c r="I11" s="2" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
+          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0</v>
+        <v>1996.4</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MEGAMAFERS S.A.</t>
+          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>1202.85</v>
+        <v>0</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>0</v>
@@ -1291,7 +1291,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
+          <t>MEGAMAFERS S.A.</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
@@ -1310,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>0</v>
+        <v>1202.85</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>0</v>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ORTEGA PAREDES RUDHT ELENA</t>
+          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OÑATE PEREZ MERCY YOLANDA</t>
+          <t>ORTEGA PAREDES RUDHT ELENA</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PADILLA MIER BERTHA MARIETA</t>
+          <t>OÑATE PEREZ MERCY YOLANDA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PAVIMARSA S.A.</t>
+          <t>PADILLA MIER BERTHA MARIETA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SARZOSA UNDA JOSE DOMINGO</t>
+          <t>PAVIMARSA S.A.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
@@ -1637,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>-1220.11</v>
+        <v>0</v>
       </c>
       <c r="R19" s="2" t="n">
         <v>0</v>
@@ -1651,7 +1651,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
+          <t>SARZOSA UNDA JOSE DOMINGO</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
@@ -1697,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="2" t="n">
-        <v>0</v>
+        <v>-1220.11</v>
       </c>
       <c r="R20" s="2" t="n">
         <v>0</v>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -1771,137 +1771,197 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>TULCAN NARVAEZ EDITH MARITZA</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="2" t="n">
+      <c r="C23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="n">
         <v>457.92</v>
       </c>
-      <c r="E22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2" t="n">
+      <c r="E23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="n">
         <v>2847.34</v>
       </c>
-      <c r="I22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" s="2" t="n">
+      <c r="I23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="n">
         <v>5082.56</v>
       </c>
-      <c r="N22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="C23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="inlineStr">
-        <is>
-          <t>1 de 21</t>
-        </is>
-      </c>
-      <c r="E23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="F23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="G23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="H23" s="4" t="inlineStr">
-        <is>
-          <t>3 de 21</t>
-        </is>
-      </c>
-      <c r="I23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="J23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="L23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="M23" s="4" t="inlineStr">
-        <is>
-          <t>2 de 21</t>
-        </is>
-      </c>
-      <c r="N23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="O23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="P23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="Q23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
-        </is>
-      </c>
-      <c r="R23" s="4" t="inlineStr">
-        <is>
-          <t>0 de 21</t>
+      <c r="N23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="inlineStr">
+        <is>
+          <t>1 de 22</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="G24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>3 de 22</t>
+        </is>
+      </c>
+      <c r="I24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="L24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="M24" s="4" t="inlineStr">
+        <is>
+          <t>2 de 22</t>
+        </is>
+      </c>
+      <c r="N24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="O24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="P24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="Q24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
+        </is>
+      </c>
+      <c r="R24" s="4" t="inlineStr">
+        <is>
+          <t>0 de 22</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1976,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2086,23 +2146,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CHASIQUIZA CAMPAÑA JOSE LUIS</t>
+          <t>CARRION CARRION STEPHANIE DAYANA</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>1392.03</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>7713.51</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>10679.6</v>
+        <v>0</v>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>4000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2113,23 +2173,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHONTASI SIMBAÑA SILVIA JANETH</t>
+          <t>CHASIQUIZA CAMPAÑA JOSE LUIS</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>109.62</v>
+        <v>1392.03</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0</v>
+        <v>7713.51</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0</v>
+        <v>10679.6</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>150.71</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>1000</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="8">
@@ -2140,11 +2200,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DECORHOME S.C.C.</t>
+          <t>CHONTASI SIMBAÑA SILVIA JANETH</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0</v>
+        <v>109.62</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>0</v>
@@ -2153,10 +2213,10 @@
         <v>0</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0</v>
+        <v>150.71</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>4000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9">
@@ -2167,7 +2227,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ESCUDERO CRUZ SILVIA RAQUEL</t>
+          <t>DECORHOME S.C.C.</t>
         </is>
       </c>
       <c r="C9" s="2" t="n">
@@ -2183,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="10">
@@ -2194,14 +2254,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FERRETERIAS FERRIGONZ SA</t>
+          <t>ESCUDERO CRUZ SILVIA RAQUEL</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>2272.64</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>507.6</v>
+        <v>0</v>
       </c>
       <c r="E10" s="2" t="n">
         <v>0</v>
@@ -2221,23 +2281,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
+          <t>FERRETERIAS FERRIGONZ SA</t>
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>6897.82</v>
+        <v>2272.64</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>5172.27</v>
+        <v>507.6</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>9948.6</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>1996.4</v>
+        <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>7000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2248,23 +2308,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
+          <t>JARAMILLO CARVAJAL NICOLAS ESTEBAN</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0</v>
+        <v>6897.82</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0</v>
+        <v>5172.27</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0</v>
+        <v>9948.6</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0</v>
+        <v>1996.4</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="13">
@@ -2275,23 +2335,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MEGAMAFERS S.A.</t>
+          <t>MATERIALES DE CONSTRUCCION SUPERMACONSVI S.A.</t>
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>14573.17</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>-494.21</v>
+        <v>0</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>12825.62</v>
+        <v>0</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>1202.85</v>
+        <v>0</v>
       </c>
       <c r="G13" s="2" t="n">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2302,23 +2362,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
+          <t>MEGAMAFERS S.A.</t>
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>11342.53</v>
+        <v>14573.17</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>4850.15</v>
+        <v>-494.21</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>9712.51</v>
+        <v>12825.62</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>0</v>
+        <v>1202.85</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>7000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="15">
@@ -2329,23 +2389,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ORTEGA PAREDES RUDHT ELENA</t>
+          <t>MUÑOZ LOZA ROMMEL SEBASTIAN</t>
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>0</v>
+        <v>11342.53</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0</v>
+        <v>4850.15</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0</v>
+        <v>9712.51</v>
       </c>
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G15" s="2" t="n">
-        <v>500</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="16">
@@ -2356,17 +2416,17 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OÑATE PEREZ MERCY YOLANDA</t>
+          <t>ORTEGA PAREDES RUDHT ELENA</t>
         </is>
       </c>
       <c r="C16" s="2" t="n">
-        <v>2350.99</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>3156.1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>2698.29</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
@@ -2383,23 +2443,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PADILLA MIER BERTHA MARIETA</t>
+          <t>OÑATE PEREZ MERCY YOLANDA</t>
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>6213.78</v>
+        <v>2350.99</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>16276.37</v>
+        <v>3156.1</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>4419.18</v>
+        <v>2698.29</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>9500</v>
+        <v>500</v>
       </c>
     </row>
     <row r="18">
@@ -2410,23 +2470,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PAVIMARSA S.A.</t>
+          <t>PADILLA MIER BERTHA MARIETA</t>
         </is>
       </c>
       <c r="C18" s="2" t="n">
-        <v>0</v>
+        <v>6213.78</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0</v>
+        <v>16276.37</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0</v>
+        <v>4419.18</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>0</v>
+        <v>9500</v>
       </c>
     </row>
     <row r="19">
@@ -2437,11 +2497,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SARZOSA UNDA JOSE DOMINGO</t>
+          <t>PAVIMARSA S.A.</t>
         </is>
       </c>
       <c r="C19" s="2" t="n">
-        <v>443.14</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>0</v>
@@ -2450,7 +2510,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="n">
-        <v>-1220.11</v>
+        <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>0</v>
@@ -2464,11 +2524,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
+          <t>SARZOSA UNDA JOSE DOMINGO</t>
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
+        <v>443.14</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>0</v>
@@ -2477,10 +2537,10 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>0</v>
+        <v>-1220.11</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -2491,7 +2551,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+          <t>SIGCHOS MORA FRANKLIN PORFIRIO</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
@@ -2507,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>2500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="22">
@@ -2518,39 +2578,66 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>TRUJILLO TORRES VINICIO RUBEN</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HIDALGO HIDALGO PEDRO GUSTAVO</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>TULCAN NARVAEZ EDITH MARITZA</t>
         </is>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C23" s="2" t="n">
         <v>10848.32</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D23" s="2" t="n">
         <v>4205.02</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E23" s="2" t="n">
         <v>13320.25</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F23" s="2" t="n">
         <v>8387.82</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G23" s="2" t="n">
         <v>6000</v>
       </c>
     </row>
-    <row r="23">
-      <c r="C23" s="6" t="n">
+    <row r="24">
+      <c r="C24" s="6" t="n">
         <v>61624.43</v>
       </c>
-      <c r="D23" s="6" t="n">
+      <c r="D24" s="6" t="n">
         <v>50808.59</v>
       </c>
-      <c r="E23" s="6" t="n">
+      <c r="E24" s="6" t="n">
         <v>66667.3</v>
       </c>
-      <c r="F23" s="6" t="n">
+      <c r="F24" s="6" t="n">
         <v>10517.67</v>
       </c>
-      <c r="G23" s="6" t="n">
+      <c r="G24" s="6" t="n">
         <v>52500</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización automática 2025-12-05 17:30:07
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="2" t="n">
-        <v>0</v>
+        <v>-52.62</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0</v>
@@ -2375,7 +2375,7 @@
         <v>12825.62</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>1202.85</v>
+        <v>1150.23</v>
       </c>
       <c r="G14" s="2" t="n">
         <v>5000</v>
@@ -2635,7 +2635,7 @@
         <v>66667.3</v>
       </c>
       <c r="F24" s="6" t="n">
-        <v>10517.67</v>
+        <v>10465.05</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>52500</v>

</xml_diff>

<commit_message>
Actualización automática 2026-01-08 14:23:39
</commit_message>
<xml_diff>
--- a/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
+++ b/data/HIDALGO HIDALGO PEDRO GUSTAVO.xlsx
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>0</v>
+        <v>908.1</v>
       </c>
       <c r="I17" s="2" t="n">
         <v>0</v>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="H25" s="4" t="inlineStr">
         <is>
-          <t>0 de 23</t>
+          <t>1 de 23</t>
         </is>
       </c>
       <c r="I25" s="4" t="inlineStr">
@@ -2516,7 +2516,7 @@
         <v>3091.73</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>0</v>
+        <v>939.4</v>
       </c>
       <c r="G17" s="2" t="n">
         <v>1500</v>
@@ -2722,7 +2722,7 @@
         <v>59467.53</v>
       </c>
       <c r="F25" s="6" t="n">
-        <v>-27</v>
+        <v>912.4</v>
       </c>
       <c r="G25" s="6" t="n">
         <v>49000</v>

</xml_diff>